<commit_message>
update session ts in recording summary
</commit_message>
<xml_diff>
--- a/inclusion_lists/recordings_summary.xlsx
+++ b/inclusion_lists/recordings_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="613">
   <si>
     <t>date</t>
   </si>
@@ -1360,9 +1360,6 @@
     <t>numTT</t>
   </si>
   <si>
-    <t>[NaN NaN;NaN NaN;NaN NaN]</t>
-  </si>
-  <si>
     <t>[33197649000 33847970000;33879776000 39654973000;39809045000 40564242000]</t>
   </si>
   <si>
@@ -1429,9 +1426,6 @@
     <t>[68567259000 69533036000;69642503000 74271356000;74356688000 74882113000]</t>
   </si>
   <si>
-    <t>[68826522000 69408005000;69483162000 71437305000;NaN NaN]</t>
-  </si>
-  <si>
     <t>[74151114000 74684897000;74764834000 79599863000;79659626000 80222027000]</t>
   </si>
   <si>
@@ -1561,9 +1555,6 @@
     <t>[26056256000 26774989000;26824522000 31013851000;31058042000 31505848000]</t>
   </si>
   <si>
-    <t>[27915698000 28583811000;28698517000 32606262000;NaN NaN]</t>
-  </si>
-  <si>
     <t>[34104711000 34394945000;34468040000 36498620000;36499762000 36969301000]</t>
   </si>
   <si>
@@ -1642,9 +1633,6 @@
     <t>[28438751000 29020884000;29083960000 35028992000;35094695000 36298695000]</t>
   </si>
   <si>
-    <t>[29697341000 30241722000;30303255000 33825613000;33885404000 34808640]</t>
-  </si>
-  <si>
     <t>[26563014000 27403273000;27848405000 33078094000;33144594000 34385221000]</t>
   </si>
   <si>
@@ -1705,10 +1693,184 @@
     <t>SpikeLog-16</t>
   </si>
   <si>
-    <t>[25644013000 26208983000;26280073000 30072736000;30146742000 30570766000]</t>
-  </si>
-  <si>
-    <t>[27080127000 27482655000;27540375000 30202957000;30283593000 ]</t>
+    <t>[29697341000 30241722000;30303255000 33825613000;33885404000 34808640000]</t>
+  </si>
+  <si>
+    <t>{'Sleep1';'Behave'}</t>
+  </si>
+  <si>
+    <t>[27915698000 28583811000;28698517000 32606262000]</t>
+  </si>
+  <si>
+    <t>[25643939000 26208910000;26280006000 30072658000;30146664000 30570691000]</t>
+  </si>
+  <si>
+    <t>[27080067000 27482581000;27540302000 30205645161;30283534000 30795093000]</t>
+  </si>
+  <si>
+    <t>[31698515000 32388958000;32451184000 35993353000;36041535000 36907582000]</t>
+  </si>
+  <si>
+    <t>[34126257000 34632968000;34685175000 37288796000;37352151000 38640705000]</t>
+  </si>
+  <si>
+    <t>[27645518000 28223735000;28282930000 32732190860;32809548000 33749065000]</t>
+  </si>
+  <si>
+    <t>[26613507000 27492562000;27550752000 32826518000;32915169000 34385383000]</t>
+  </si>
+  <si>
+    <t>[27221440000 27973762000;28032406000 32243754210;32317057518 33599647000]</t>
+  </si>
+  <si>
+    <t>[28171083000 28728855000;28778759000 31906505000;31949233000 32530761000]</t>
+  </si>
+  <si>
+    <t>[32918784000 33544532000;33608642000 36430648000;36486980000 37024379000]</t>
+  </si>
+  <si>
+    <t>[40017903000 40559645000;40600699000 43102710000;43147232000 43791828000]</t>
+  </si>
+  <si>
+    <t>[27515720000 28115145000;28159623000 31625408000;31678157000 32411503000]</t>
+  </si>
+  <si>
+    <t>[35113647000 35833464000;35997508000 38886907000;38948954000 39566061000]</t>
+  </si>
+  <si>
+    <t>[34115607000 34702468000;34750972000 36977766000;37041843000 37659491000]</t>
+  </si>
+  <si>
+    <t>[29658125000 30322010000;30365423000 32998092000;33059440000 33758578000]</t>
+  </si>
+  <si>
+    <t>[26406026000 27078860000;27130964000 30472670000;30548245000 31166521000]</t>
+  </si>
+  <si>
+    <t>[33492933000 34187014000;34241180000 37463687000;37525844000 38190537000]</t>
+  </si>
+  <si>
+    <t>[27725631000 28484090000;28583314000 32240082000;32299224000 33036536000]</t>
+  </si>
+  <si>
+    <t>[31883474000 32475050000;32529951000 35631837000;35705759000 36958790000]</t>
+  </si>
+  <si>
+    <t>[25390075000 26066280000;26157536000 30599940000;30664420000 32037325000]</t>
+  </si>
+  <si>
+    <t>[35075875000 35673503000;35741879000 39341969000;39399140000 40074065000]</t>
+  </si>
+  <si>
+    <t>[29694462000 30360727000;30420460000 33453590000;33528477000 34432277000]</t>
+  </si>
+  <si>
+    <t>[33522006000 34065747000;34120048000 37006776000;37078376000 37753233000]</t>
+  </si>
+  <si>
+    <t>[33829611000 34391615000;34438865000 37073073000;37279612000 37954063000]</t>
+  </si>
+  <si>
+    <t>[26042538000 26609248000;26661590000 31842413000;31944710000 32622461000]</t>
+  </si>
+  <si>
+    <t>[25974691000 26765918000;26837338000 30428169000;30493622000 31284180000]</t>
+  </si>
+  <si>
+    <t>[25712024000 26656676000;26805060000 30859688000;30932418000 31734909000]</t>
+  </si>
+  <si>
+    <t>[26861012000 27565075000;27634517000 31798970000;31846790000 32476354000]</t>
+  </si>
+  <si>
+    <t>[25314295000 26028965000;26077187000 30459415000;30532318000 31270800000]</t>
+  </si>
+  <si>
+    <t>[57060029000 57723030000;57827429000 61244017000;61504482000 62171980000]</t>
+  </si>
+  <si>
+    <t>[52550829000 53539437000;53683464000 57971815000;58189031000 58957190000]</t>
+  </si>
+  <si>
+    <t>[60383186000 61496060000;61601833000 63165486000;63445997000 64095982000]</t>
+  </si>
+  <si>
+    <t>[68826522000 69408005000;69483162000 71437305000]</t>
+  </si>
+  <si>
+    <t>[67444814000 68085219000;68206184000 69686620000;69689255000 69940845000]</t>
+  </si>
+  <si>
+    <t>[68711730000 69528972000;69593207000 72492190000;72617636000 73315995000]</t>
+  </si>
+  <si>
+    <t>[63245086000 63864197000;63965865000 69671972000;69677255000 70379927000]</t>
+  </si>
+  <si>
+    <t>[63223316000 64017539000;64033917000 69564256000;69729672000 70414079000]</t>
+  </si>
+  <si>
+    <t>[63833799000 64476471000;64532093000 70560793000;70565520000 71012996000]</t>
+  </si>
+  <si>
+    <t>[30099119000 31083112000;31143408000 36163108000;36290075000 37231771000]</t>
+  </si>
+  <si>
+    <t>[60243542000 60962179000;60996153000 66774130000;66919774000 67500534000]</t>
+  </si>
+  <si>
+    <t>[33434773000 34049496000;34097645000 39811708000;39931290000 40608677000]</t>
+  </si>
+  <si>
+    <t>[66755351000 67406779000;67424562000 73193515000;73452573000 73963274000]</t>
+  </si>
+  <si>
+    <t>[60996357000 61867477000;62157417000 67168889000;67310536000 68164343000]</t>
+  </si>
+  <si>
+    <t>[33803119000 34471105000;34528644000 40086826000;40255397000 41017383000]</t>
+  </si>
+  <si>
+    <t>[33576211000 34187675000;34238197000 39682795000;39832166000 40600295000]</t>
+  </si>
+  <si>
+    <t>there were sirens (PIKUD HAOREF) during Sleep2</t>
+  </si>
+  <si>
+    <t>[33863629000 34487538000;34536558000 39783756000;39971989000 40858836000]</t>
+  </si>
+  <si>
+    <t>[34215219000 34912469000;34989973000 40562398000;40714233000 41458166000]</t>
+  </si>
+  <si>
+    <t>[33473273000 34187879000;34218951000 39867665000;39945084000 40738527000]</t>
+  </si>
+  <si>
+    <t>during one of the flights the bat ate some banana piece! (check for artifacts/different coding during this flight…)</t>
+  </si>
+  <si>
+    <t>[33280287000 34043565000;34323895000 39701807000;39866390000 40623120000]</t>
+  </si>
+  <si>
+    <t>[33671718000 34310159000;34367201049 39545901000;39729291000 40458720000]</t>
+  </si>
+  <si>
+    <t>[33198953000 33899791000;33958915000 38929148000;38953043000 39760749000]</t>
+  </si>
+  <si>
+    <t>[34660953000 35263685000;35320331000 38387656000;38553093000 39047194000]</t>
+  </si>
+  <si>
+    <t>[33689905000 34354626000;34433215000 37737742000;37888626000 38737995000]</t>
+  </si>
+  <si>
+    <t>[34982702000 35589078000;35619665000 39680884000;39808319000 40492917000]</t>
+  </si>
+  <si>
+    <t>[32787408000 33325992000;33387730000 37088798000;37184588000 37572495000]</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -2468,23 +2630,23 @@
   <dimension ref="A1:Z174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K140" sqref="K140"/>
+      <selection pane="bottomRight" activeCell="J144" sqref="J144:K144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.625" customWidth="1"/>
-    <col min="8" max="8" width="7.5" customWidth="1"/>
-    <col min="9" max="9" width="6.75" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="2" max="2" width="4.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
+    <col min="8" max="8" width="5.625" customWidth="1"/>
+    <col min="9" max="9" width="5.875" customWidth="1"/>
+    <col min="10" max="10" width="24.625" customWidth="1"/>
     <col min="11" max="11" width="74.25" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.75" customWidth="1"/>
     <col min="13" max="13" width="2.5" customWidth="1"/>
@@ -2492,7 +2654,8 @@
     <col min="15" max="15" width="3.75" customWidth="1"/>
     <col min="16" max="16" width="3.25" customWidth="1"/>
     <col min="17" max="17" width="3.125" customWidth="1"/>
-    <col min="18" max="19" width="5.375" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="3.5" customWidth="1"/>
     <col min="20" max="20" width="3" customWidth="1"/>
     <col min="21" max="21" width="5.125" customWidth="1"/>
     <col min="22" max="22" width="4" customWidth="1"/>
@@ -2502,21 +2665,21 @@
     <col min="26" max="26" width="78.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="199.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>441</v>
@@ -2525,16 +2688,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>108</v>
@@ -2546,19 +2709,19 @@
         <v>229</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>109</v>
@@ -2567,19 +2730,19 @@
         <v>46</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -2605,10 +2768,7 @@
         <v>44</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2637,10 +2797,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2666,10 +2823,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -2695,10 +2849,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -2724,10 +2875,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -2753,10 +2901,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -2782,10 +2927,7 @@
         <v>4</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -2811,10 +2953,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -2840,10 +2979,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -2869,10 +3005,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2898,10 +3031,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -2927,10 +3057,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2956,10 +3083,7 @@
         <v>4</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -2985,10 +3109,7 @@
         <v>4</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -3014,10 +3135,7 @@
         <v>4</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -3026,7 +3144,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>80</v>
       </c>
@@ -3043,10 +3161,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -3055,7 +3170,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>81</v>
       </c>
@@ -3072,10 +3187,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -3084,7 +3196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -3101,10 +3213,7 @@
         <v>4</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -3113,7 +3222,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
@@ -3130,10 +3239,7 @@
         <v>4</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>442</v>
+        <v>549</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -3142,7 +3248,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -3168,10 +3274,16 @@
         <v>146</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>553</v>
+        <v>612</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>442</v>
+        <v>128</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -3183,7 +3295,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
@@ -3209,10 +3321,16 @@
         <v>146</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>553</v>
+        <v>612</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>442</v>
+        <v>128</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -3224,7 +3342,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -3250,10 +3368,10 @@
         <v>146</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>442</v>
+        <v>611</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -3262,7 +3380,7 @@
         <v>45</v>
       </c>
       <c r="S23" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T23">
         <v>14</v>
@@ -3271,7 +3389,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -3297,10 +3415,10 @@
         <v>146</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>442</v>
+        <v>610</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -3309,7 +3427,7 @@
         <v>45</v>
       </c>
       <c r="S24" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T24">
         <v>14</v>
@@ -3318,7 +3436,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -3344,10 +3462,10 @@
         <v>146</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>442</v>
+        <v>609</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -3356,7 +3474,7 @@
         <v>45</v>
       </c>
       <c r="S25" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T25">
         <v>14</v>
@@ -3365,7 +3483,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -3391,10 +3509,10 @@
         <v>146</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>442</v>
+        <v>608</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -3403,7 +3521,7 @@
         <v>45</v>
       </c>
       <c r="S26" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T26">
         <v>14</v>
@@ -3412,7 +3530,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
@@ -3438,10 +3556,10 @@
         <v>146</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>442</v>
+        <v>607</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -3450,7 +3568,7 @@
         <v>45</v>
       </c>
       <c r="S27" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T27">
         <v>14</v>
@@ -3459,7 +3577,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -3485,10 +3603,10 @@
         <v>146</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>442</v>
+        <v>606</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -3497,7 +3615,7 @@
         <v>45</v>
       </c>
       <c r="S28" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T28">
         <v>14</v>
@@ -3506,7 +3624,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -3532,10 +3650,10 @@
         <v>146</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="L29">
         <v>1</v>
@@ -3559,7 +3677,7 @@
         <v>45</v>
       </c>
       <c r="S29" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T29">
         <v>14</v>
@@ -3568,7 +3686,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -3594,10 +3712,10 @@
         <v>146</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>442</v>
+        <v>605</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -3606,7 +3724,7 @@
         <v>45</v>
       </c>
       <c r="S30" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T30">
         <v>14</v>
@@ -3615,7 +3733,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -3641,10 +3759,10 @@
         <v>146</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>442</v>
+        <v>603</v>
       </c>
       <c r="N31">
         <v>0</v>
@@ -3653,7 +3771,7 @@
         <v>45</v>
       </c>
       <c r="S31" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T31">
         <v>14</v>
@@ -3661,8 +3779,11 @@
       <c r="U31">
         <v>3089</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="X31" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -3688,10 +3809,10 @@
         <v>146</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>442</v>
+        <v>602</v>
       </c>
       <c r="N32">
         <v>0</v>
@@ -3700,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="S32" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T32">
         <v>14</v>
@@ -3735,10 +3856,10 @@
         <v>146</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>442</v>
+        <v>601</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -3747,7 +3868,7 @@
         <v>45</v>
       </c>
       <c r="S33" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T33">
         <v>14</v>
@@ -3782,10 +3903,10 @@
         <v>146</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L34">
         <v>1</v>
@@ -3809,7 +3930,7 @@
         <v>45</v>
       </c>
       <c r="S34" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T34">
         <v>14</v>
@@ -3844,10 +3965,10 @@
         <v>146</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>442</v>
+        <v>599</v>
       </c>
       <c r="N35">
         <v>0</v>
@@ -3856,13 +3977,16 @@
         <v>45</v>
       </c>
       <c r="S35" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T35">
         <v>14</v>
       </c>
       <c r="U35">
         <v>3089</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
@@ -3891,10 +4015,10 @@
         <v>146</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>442</v>
+        <v>598</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -3903,7 +4027,7 @@
         <v>45</v>
       </c>
       <c r="S36" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T36">
         <v>14</v>
@@ -3938,10 +4062,10 @@
         <v>146</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>442</v>
+        <v>597</v>
       </c>
       <c r="N37">
         <v>0</v>
@@ -3950,7 +4074,7 @@
         <v>45</v>
       </c>
       <c r="S37" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T37">
         <v>14</v>
@@ -3985,10 +4109,10 @@
         <v>146</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>442</v>
+        <v>596</v>
       </c>
       <c r="N38">
         <v>0</v>
@@ -3997,7 +4121,7 @@
         <v>45</v>
       </c>
       <c r="S38" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T38">
         <v>14</v>
@@ -4032,10 +4156,10 @@
         <v>146</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>442</v>
+        <v>595</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -4044,7 +4168,7 @@
         <v>45</v>
       </c>
       <c r="S39" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T39">
         <v>14</v>
@@ -4079,10 +4203,10 @@
         <v>146</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L40">
         <v>1</v>
@@ -4106,7 +4230,7 @@
         <v>45</v>
       </c>
       <c r="S40" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T40">
         <v>14</v>
@@ -4141,10 +4265,10 @@
         <v>146</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>442</v>
+        <v>594</v>
       </c>
       <c r="N41">
         <v>0</v>
@@ -4153,7 +4277,7 @@
         <v>45</v>
       </c>
       <c r="S41" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T41">
         <v>14</v>
@@ -4188,10 +4312,10 @@
         <v>146</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="L42">
         <v>1</v>
@@ -4215,7 +4339,7 @@
         <v>45</v>
       </c>
       <c r="S42" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T42">
         <v>14</v>
@@ -4250,10 +4374,10 @@
         <v>146</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -4277,7 +4401,7 @@
         <v>45</v>
       </c>
       <c r="S43" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T43">
         <v>14</v>
@@ -4312,10 +4436,10 @@
         <v>146</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>442</v>
+        <v>593</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -4324,7 +4448,7 @@
         <v>45</v>
       </c>
       <c r="S44" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T44">
         <v>14</v>
@@ -4359,10 +4483,10 @@
         <v>146</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>442</v>
+        <v>592</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -4371,7 +4495,7 @@
         <v>45</v>
       </c>
       <c r="S45" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T45">
         <v>14</v>
@@ -4406,10 +4530,10 @@
         <v>146</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>442</v>
+        <v>591</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -4418,7 +4542,7 @@
         <v>45</v>
       </c>
       <c r="S46" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T46">
         <v>14</v>
@@ -4453,10 +4577,10 @@
         <v>146</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>442</v>
+        <v>590</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -4465,7 +4589,7 @@
         <v>45</v>
       </c>
       <c r="S47" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T47">
         <v>14</v>
@@ -4500,10 +4624,10 @@
         <v>130</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>553</v>
+        <v>612</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>442</v>
+        <v>128</v>
       </c>
       <c r="L48">
         <v>1</v>
@@ -4527,7 +4651,7 @@
         <v>45</v>
       </c>
       <c r="S48" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T48">
         <v>14</v>
@@ -4571,10 +4695,10 @@
         <v>130</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L49">
         <v>1</v>
@@ -4598,7 +4722,7 @@
         <v>45</v>
       </c>
       <c r="S49" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T49">
         <v>14</v>
@@ -4639,10 +4763,10 @@
         <v>130</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K50" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L50">
         <v>1</v>
@@ -4666,7 +4790,7 @@
         <v>45</v>
       </c>
       <c r="S50" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T50">
         <v>14</v>
@@ -4707,10 +4831,10 @@
         <v>130</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L51">
         <v>1</v>
@@ -4734,7 +4858,7 @@
         <v>45</v>
       </c>
       <c r="S51" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T51">
         <v>14</v>
@@ -4775,10 +4899,10 @@
         <v>130</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>442</v>
+        <v>589</v>
       </c>
       <c r="L52">
         <v>1</v>
@@ -4802,7 +4926,7 @@
         <v>45</v>
       </c>
       <c r="S52" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T52">
         <v>14</v>
@@ -4843,10 +4967,10 @@
         <v>130</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L53">
         <v>1</v>
@@ -4870,7 +4994,7 @@
         <v>45</v>
       </c>
       <c r="S53" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T53">
         <v>14</v>
@@ -4911,10 +5035,10 @@
         <v>130</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L54">
         <v>1</v>
@@ -4938,7 +5062,7 @@
         <v>45</v>
       </c>
       <c r="S54" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T54">
         <v>14</v>
@@ -4979,10 +5103,10 @@
         <v>130</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="L55">
         <v>1</v>
@@ -5006,7 +5130,7 @@
         <v>45</v>
       </c>
       <c r="S55" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T55">
         <v>14</v>
@@ -5047,10 +5171,10 @@
         <v>131</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L56">
         <v>1</v>
@@ -5074,7 +5198,7 @@
         <v>45</v>
       </c>
       <c r="S56" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T56">
         <v>14</v>
@@ -5115,10 +5239,10 @@
         <v>130</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="L57">
         <v>1</v>
@@ -5142,7 +5266,7 @@
         <v>45</v>
       </c>
       <c r="S57" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T57">
         <v>14</v>
@@ -5183,10 +5307,10 @@
         <v>130</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L58">
         <v>1</v>
@@ -5210,7 +5334,7 @@
         <v>45</v>
       </c>
       <c r="S58" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T58">
         <v>14</v>
@@ -5251,10 +5375,10 @@
         <v>130</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L59">
         <v>1</v>
@@ -5278,7 +5402,7 @@
         <v>45</v>
       </c>
       <c r="S59" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T59">
         <v>14</v>
@@ -5319,10 +5443,10 @@
         <v>130</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="L60">
         <v>1</v>
@@ -5346,7 +5470,7 @@
         <v>45</v>
       </c>
       <c r="S60" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T60">
         <v>14</v>
@@ -5387,10 +5511,10 @@
         <v>130</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L61">
         <v>1</v>
@@ -5414,7 +5538,7 @@
         <v>45</v>
       </c>
       <c r="S61" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T61">
         <v>14</v>
@@ -5455,10 +5579,10 @@
         <v>130</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="L62">
         <v>1</v>
@@ -5482,7 +5606,7 @@
         <v>45</v>
       </c>
       <c r="S62" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T62">
         <v>14</v>
@@ -5523,10 +5647,10 @@
         <v>130</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L63">
         <v>1</v>
@@ -5550,7 +5674,7 @@
         <v>45</v>
       </c>
       <c r="S63" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T63">
         <v>14</v>
@@ -5591,10 +5715,10 @@
         <v>130</v>
       </c>
       <c r="J64" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L64">
         <v>1</v>
@@ -5618,7 +5742,7 @@
         <v>45</v>
       </c>
       <c r="S64" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T64">
         <v>14</v>
@@ -5659,10 +5783,10 @@
         <v>130</v>
       </c>
       <c r="J65" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="L65">
         <v>1</v>
@@ -5686,7 +5810,7 @@
         <v>45</v>
       </c>
       <c r="S65" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T65">
         <v>14</v>
@@ -5727,10 +5851,10 @@
         <v>130</v>
       </c>
       <c r="J66" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L66">
         <v>1</v>
@@ -5754,7 +5878,7 @@
         <v>45</v>
       </c>
       <c r="S66" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T66">
         <v>14</v>
@@ -5795,10 +5919,10 @@
         <v>130</v>
       </c>
       <c r="J67" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>442</v>
+        <v>588</v>
       </c>
       <c r="L67">
         <v>1</v>
@@ -5822,7 +5946,7 @@
         <v>45</v>
       </c>
       <c r="S67" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T67">
         <v>14</v>
@@ -5863,10 +5987,10 @@
         <v>130</v>
       </c>
       <c r="J68" s="13" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>465</v>
+        <v>587</v>
       </c>
       <c r="L68">
         <v>1</v>
@@ -5890,7 +6014,7 @@
         <v>45</v>
       </c>
       <c r="S68" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T68">
         <v>14</v>
@@ -5931,10 +6055,10 @@
         <v>130</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>553</v>
+        <v>612</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>442</v>
+        <v>128</v>
       </c>
       <c r="L69">
         <v>1</v>
@@ -5949,7 +6073,7 @@
         <v>170</v>
       </c>
       <c r="S69" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T69">
         <v>14</v>
@@ -5987,10 +6111,10 @@
         <v>130</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L70">
         <v>1</v>
@@ -6014,7 +6138,7 @@
         <v>45</v>
       </c>
       <c r="S70" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T70">
         <v>14</v>
@@ -6055,10 +6179,10 @@
         <v>130</v>
       </c>
       <c r="J71" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L71">
         <v>1</v>
@@ -6082,7 +6206,7 @@
         <v>45</v>
       </c>
       <c r="S71" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T71">
         <v>14</v>
@@ -6123,10 +6247,10 @@
         <v>130</v>
       </c>
       <c r="J72" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="L72">
         <v>1</v>
@@ -6150,7 +6274,7 @@
         <v>45</v>
       </c>
       <c r="S72" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T72">
         <v>14</v>
@@ -6194,10 +6318,10 @@
         <v>130</v>
       </c>
       <c r="J73" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L73">
         <v>1</v>
@@ -6221,7 +6345,7 @@
         <v>45</v>
       </c>
       <c r="S73" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T73">
         <v>14</v>
@@ -6265,10 +6389,10 @@
         <v>130</v>
       </c>
       <c r="J74" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="L74">
         <v>1</v>
@@ -6292,7 +6416,7 @@
         <v>45</v>
       </c>
       <c r="S74" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T74">
         <v>14</v>
@@ -6333,10 +6457,10 @@
         <v>130</v>
       </c>
       <c r="J75" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K75" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L75">
         <v>1</v>
@@ -6360,7 +6484,7 @@
         <v>45</v>
       </c>
       <c r="S75" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T75">
         <v>14</v>
@@ -6404,10 +6528,10 @@
         <v>130</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="L76">
         <v>1</v>
@@ -6431,7 +6555,7 @@
         <v>45</v>
       </c>
       <c r="S76" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T76">
         <v>14</v>
@@ -6472,10 +6596,10 @@
         <v>130</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="L77">
         <v>1</v>
@@ -6499,7 +6623,7 @@
         <v>45</v>
       </c>
       <c r="S77" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T77">
         <v>14</v>
@@ -6540,10 +6664,10 @@
         <v>130</v>
       </c>
       <c r="J78" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L78">
         <v>1</v>
@@ -6567,7 +6691,7 @@
         <v>45</v>
       </c>
       <c r="S78" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T78">
         <v>14</v>
@@ -6608,10 +6732,10 @@
         <v>130</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K79" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L79">
         <v>1</v>
@@ -6635,7 +6759,7 @@
         <v>45</v>
       </c>
       <c r="S79" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T79">
         <v>14</v>
@@ -6676,10 +6800,10 @@
         <v>130</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K80" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="L80">
         <v>1</v>
@@ -6703,7 +6827,7 @@
         <v>45</v>
       </c>
       <c r="S80" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T80">
         <v>14</v>
@@ -6744,10 +6868,10 @@
         <v>130</v>
       </c>
       <c r="J81" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K81" s="12" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L81">
         <v>1</v>
@@ -6771,7 +6895,7 @@
         <v>45</v>
       </c>
       <c r="S81" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T81">
         <v>14</v>
@@ -6815,10 +6939,10 @@
         <v>130</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K82" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="L82">
         <v>1</v>
@@ -6842,7 +6966,7 @@
         <v>45</v>
       </c>
       <c r="S82" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T82">
         <v>14</v>
@@ -6883,10 +7007,10 @@
         <v>130</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K83" s="12" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="L83">
         <v>1</v>
@@ -6910,7 +7034,7 @@
         <v>45</v>
       </c>
       <c r="S83" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T83">
         <v>14</v>
@@ -6954,10 +7078,10 @@
         <v>44</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K84" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="L84">
         <v>1</v>
@@ -6981,7 +7105,7 @@
         <v>45</v>
       </c>
       <c r="S84" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T84">
         <v>5</v>
@@ -7022,10 +7146,10 @@
         <v>44</v>
       </c>
       <c r="J85" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K85" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L85">
         <v>1</v>
@@ -7049,7 +7173,7 @@
         <v>45</v>
       </c>
       <c r="S85" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T85">
         <v>5</v>
@@ -7093,10 +7217,10 @@
         <v>44</v>
       </c>
       <c r="J86" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K86" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L86">
         <v>1</v>
@@ -7120,7 +7244,7 @@
         <v>45</v>
       </c>
       <c r="S86" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T86">
         <v>5</v>
@@ -7164,10 +7288,10 @@
         <v>44</v>
       </c>
       <c r="J87" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K87" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L87">
         <v>1</v>
@@ -7191,7 +7315,7 @@
         <v>45</v>
       </c>
       <c r="S87" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T87">
         <v>5</v>
@@ -7235,10 +7359,10 @@
         <v>44</v>
       </c>
       <c r="J88" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K88" s="12" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="L88">
         <v>1</v>
@@ -7262,7 +7386,7 @@
         <v>45</v>
       </c>
       <c r="S88" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T88">
         <v>5</v>
@@ -7306,10 +7430,10 @@
         <v>44</v>
       </c>
       <c r="J89" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K89" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="L89">
         <v>1</v>
@@ -7333,7 +7457,7 @@
         <v>45</v>
       </c>
       <c r="S89" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T89">
         <v>5</v>
@@ -7377,10 +7501,10 @@
         <v>44</v>
       </c>
       <c r="J90" s="13" t="s">
-        <v>553</v>
+        <v>612</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>442</v>
+        <v>128</v>
       </c>
       <c r="L90">
         <v>0</v>
@@ -7404,7 +7528,7 @@
         <v>45</v>
       </c>
       <c r="S90" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T90">
         <v>5</v>
@@ -7448,10 +7572,10 @@
         <v>44</v>
       </c>
       <c r="J91" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K91" s="12" t="s">
-        <v>442</v>
+        <v>586</v>
       </c>
       <c r="L91">
         <v>1</v>
@@ -7475,7 +7599,7 @@
         <v>45</v>
       </c>
       <c r="S91" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T91">
         <v>5</v>
@@ -7519,10 +7643,10 @@
         <v>44</v>
       </c>
       <c r="J92" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K92" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="L92">
         <v>1</v>
@@ -7546,7 +7670,7 @@
         <v>45</v>
       </c>
       <c r="S92" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T92">
         <v>5</v>
@@ -7590,10 +7714,10 @@
         <v>44</v>
       </c>
       <c r="J93" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K93" s="12" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="L93">
         <v>1</v>
@@ -7617,7 +7741,7 @@
         <v>45</v>
       </c>
       <c r="S93" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T93">
         <v>5</v>
@@ -7661,10 +7785,10 @@
         <v>44</v>
       </c>
       <c r="J94" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K94" s="12" t="s">
-        <v>442</v>
+        <v>585</v>
       </c>
       <c r="L94">
         <v>1</v>
@@ -7688,7 +7812,7 @@
         <v>45</v>
       </c>
       <c r="S94" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T94">
         <v>5</v>
@@ -7732,10 +7856,10 @@
         <v>44</v>
       </c>
       <c r="J95" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K95" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="L95">
         <v>1</v>
@@ -7759,7 +7883,7 @@
         <v>45</v>
       </c>
       <c r="S95" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T95">
         <v>5</v>
@@ -7803,10 +7927,10 @@
         <v>44</v>
       </c>
       <c r="J96" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K96" s="12" t="s">
-        <v>442</v>
+        <v>584</v>
       </c>
       <c r="L96">
         <v>1</v>
@@ -7830,7 +7954,7 @@
         <v>45</v>
       </c>
       <c r="S96" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T96">
         <v>5</v>
@@ -7874,10 +7998,10 @@
         <v>44</v>
       </c>
       <c r="J97" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K97" s="12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="L97">
         <v>1</v>
@@ -7901,7 +8025,7 @@
         <v>45</v>
       </c>
       <c r="S97" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T97">
         <v>5</v>
@@ -7945,10 +8069,10 @@
         <v>44</v>
       </c>
       <c r="J98" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K98" s="12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="L98">
         <v>1</v>
@@ -7972,7 +8096,7 @@
         <v>45</v>
       </c>
       <c r="S98" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T98">
         <v>5</v>
@@ -8016,10 +8140,10 @@
         <v>44</v>
       </c>
       <c r="J99" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K99" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L99">
         <v>1</v>
@@ -8043,7 +8167,7 @@
         <v>45</v>
       </c>
       <c r="S99" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T99">
         <v>5</v>
@@ -8084,10 +8208,10 @@
         <v>44</v>
       </c>
       <c r="J100" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K100" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="L100">
         <v>1</v>
@@ -8111,7 +8235,7 @@
         <v>45</v>
       </c>
       <c r="S100" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T100">
         <v>5</v>
@@ -8155,10 +8279,10 @@
         <v>44</v>
       </c>
       <c r="J101" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K101" s="12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L101">
         <v>1</v>
@@ -8182,7 +8306,7 @@
         <v>45</v>
       </c>
       <c r="S101" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T101">
         <v>5</v>
@@ -8223,10 +8347,10 @@
         <v>44</v>
       </c>
       <c r="J102" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K102" s="12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="L102">
         <v>1</v>
@@ -8250,7 +8374,7 @@
         <v>45</v>
       </c>
       <c r="S102" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T102">
         <v>5</v>
@@ -8291,10 +8415,10 @@
         <v>44</v>
       </c>
       <c r="J103" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K103" s="12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="L103">
         <v>1</v>
@@ -8318,7 +8442,7 @@
         <v>45</v>
       </c>
       <c r="S103" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T103">
         <v>5</v>
@@ -8359,10 +8483,10 @@
         <v>44</v>
       </c>
       <c r="J104" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K104" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="L104">
         <v>1</v>
@@ -8386,7 +8510,7 @@
         <v>45</v>
       </c>
       <c r="S104" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T104">
         <v>5</v>
@@ -8427,10 +8551,10 @@
         <v>44</v>
       </c>
       <c r="J105" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K105" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="L105">
         <v>1</v>
@@ -8454,7 +8578,7 @@
         <v>45</v>
       </c>
       <c r="S105" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T105">
         <v>5</v>
@@ -8495,10 +8619,10 @@
         <v>44</v>
       </c>
       <c r="J106" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K106" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="L106">
         <v>1</v>
@@ -8522,7 +8646,7 @@
         <v>45</v>
       </c>
       <c r="S106" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T106">
         <v>5</v>
@@ -8563,10 +8687,10 @@
         <v>44</v>
       </c>
       <c r="J107" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K107" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="L107">
         <v>1</v>
@@ -8590,7 +8714,7 @@
         <v>45</v>
       </c>
       <c r="S107" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T107">
         <v>5</v>
@@ -8631,10 +8755,10 @@
         <v>44</v>
       </c>
       <c r="J108" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K108" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="L108">
         <v>1</v>
@@ -8658,7 +8782,7 @@
         <v>45</v>
       </c>
       <c r="S108" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T108">
         <v>5</v>
@@ -8699,10 +8823,10 @@
         <v>44</v>
       </c>
       <c r="J109" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K109" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="L109">
         <v>1</v>
@@ -8726,7 +8850,7 @@
         <v>45</v>
       </c>
       <c r="S109" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T109">
         <v>5</v>
@@ -8770,10 +8894,10 @@
         <v>44</v>
       </c>
       <c r="J110" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K110" s="12" t="s">
-        <v>442</v>
+        <v>583</v>
       </c>
       <c r="L110">
         <v>1</v>
@@ -8797,7 +8921,7 @@
         <v>45</v>
       </c>
       <c r="S110" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T110">
         <v>5</v>
@@ -8841,10 +8965,10 @@
         <v>44</v>
       </c>
       <c r="J111" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K111" s="12" t="s">
-        <v>442</v>
+        <v>581</v>
       </c>
       <c r="L111">
         <v>1</v>
@@ -8868,7 +8992,7 @@
         <v>45</v>
       </c>
       <c r="S111" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T111">
         <v>5</v>
@@ -8909,10 +9033,10 @@
         <v>44</v>
       </c>
       <c r="J112" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K112" s="12" t="s">
-        <v>442</v>
+        <v>582</v>
       </c>
       <c r="L112">
         <v>1</v>
@@ -8936,7 +9060,7 @@
         <v>45</v>
       </c>
       <c r="S112" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T112">
         <v>5</v>
@@ -8974,10 +9098,10 @@
         <v>44</v>
       </c>
       <c r="J113" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K113" s="12" t="s">
-        <v>442</v>
+        <v>580</v>
       </c>
       <c r="L113">
         <v>1</v>
@@ -9001,7 +9125,7 @@
         <v>45</v>
       </c>
       <c r="S113" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T113">
         <v>5</v>
@@ -9042,10 +9166,10 @@
         <v>44</v>
       </c>
       <c r="J114" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K114" s="12" t="s">
-        <v>442</v>
+        <v>579</v>
       </c>
       <c r="L114">
         <v>1</v>
@@ -9069,7 +9193,7 @@
         <v>45</v>
       </c>
       <c r="S114" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T114">
         <v>5</v>
@@ -9110,10 +9234,10 @@
         <v>44</v>
       </c>
       <c r="J115" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K115" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="L115">
         <v>1</v>
@@ -9137,7 +9261,7 @@
         <v>45</v>
       </c>
       <c r="S115" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T115">
         <v>5</v>
@@ -9178,10 +9302,10 @@
         <v>44</v>
       </c>
       <c r="J116" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K116" s="12" t="s">
-        <v>442</v>
+        <v>578</v>
       </c>
       <c r="L116">
         <v>1</v>
@@ -9205,7 +9329,7 @@
         <v>45</v>
       </c>
       <c r="S116" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T116">
         <v>4</v>
@@ -9246,10 +9370,10 @@
         <v>44</v>
       </c>
       <c r="J117" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K117" s="12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L117">
         <v>1</v>
@@ -9273,7 +9397,7 @@
         <v>45</v>
       </c>
       <c r="S117" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T117">
         <v>5</v>
@@ -9314,10 +9438,10 @@
         <v>44</v>
       </c>
       <c r="J118" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K118" s="12" t="s">
-        <v>442</v>
+        <v>577</v>
       </c>
       <c r="L118">
         <v>1</v>
@@ -9341,7 +9465,7 @@
         <v>45</v>
       </c>
       <c r="S118" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T118">
         <v>4</v>
@@ -9382,10 +9506,10 @@
         <v>44</v>
       </c>
       <c r="J119" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K119" s="12" t="s">
-        <v>442</v>
+        <v>576</v>
       </c>
       <c r="L119">
         <v>1</v>
@@ -9409,7 +9533,7 @@
         <v>45</v>
       </c>
       <c r="S119" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T119">
         <v>5</v>
@@ -9450,10 +9574,10 @@
         <v>44</v>
       </c>
       <c r="J120" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K120" s="12" t="s">
-        <v>442</v>
+        <v>575</v>
       </c>
       <c r="L120">
         <v>1</v>
@@ -9477,7 +9601,7 @@
         <v>45</v>
       </c>
       <c r="S120" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T120">
         <v>4</v>
@@ -9518,10 +9642,10 @@
         <v>44</v>
       </c>
       <c r="J121" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K121" s="12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="L121">
         <v>1</v>
@@ -9545,7 +9669,7 @@
         <v>45</v>
       </c>
       <c r="S121" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T121">
         <v>5</v>
@@ -9586,10 +9710,10 @@
         <v>44</v>
       </c>
       <c r="J122" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K122" s="12" t="s">
-        <v>442</v>
+        <v>574</v>
       </c>
       <c r="L122">
         <v>1</v>
@@ -9613,7 +9737,7 @@
         <v>45</v>
       </c>
       <c r="S122" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T122">
         <v>5</v>
@@ -9654,10 +9778,10 @@
         <v>44</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K123" s="12" t="s">
-        <v>442</v>
+        <v>573</v>
       </c>
       <c r="L123">
         <v>1</v>
@@ -9681,7 +9805,7 @@
         <v>45</v>
       </c>
       <c r="S123" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T123">
         <v>5</v>
@@ -9722,10 +9846,10 @@
         <v>44</v>
       </c>
       <c r="J124" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K124" s="12" t="s">
-        <v>442</v>
+        <v>572</v>
       </c>
       <c r="L124">
         <v>1</v>
@@ -9749,7 +9873,7 @@
         <v>45</v>
       </c>
       <c r="S124" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T124">
         <v>5</v>
@@ -9787,10 +9911,10 @@
         <v>44</v>
       </c>
       <c r="J125" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K125" s="12" t="s">
-        <v>442</v>
+        <v>571</v>
       </c>
       <c r="L125">
         <v>1</v>
@@ -9814,7 +9938,7 @@
         <v>45</v>
       </c>
       <c r="S125" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T125">
         <v>4</v>
@@ -9852,10 +9976,10 @@
         <v>44</v>
       </c>
       <c r="J126" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K126" s="12" t="s">
-        <v>442</v>
+        <v>570</v>
       </c>
       <c r="L126">
         <v>1</v>
@@ -9879,7 +10003,7 @@
         <v>45</v>
       </c>
       <c r="S126" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T126">
         <v>5</v>
@@ -9917,10 +10041,10 @@
         <v>44</v>
       </c>
       <c r="J127" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K127" s="12" t="s">
-        <v>442</v>
+        <v>569</v>
       </c>
       <c r="L127">
         <v>1</v>
@@ -9944,7 +10068,7 @@
         <v>45</v>
       </c>
       <c r="S127" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T127">
         <v>5</v>
@@ -9982,10 +10106,10 @@
         <v>44</v>
       </c>
       <c r="J128" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K128" s="12" t="s">
-        <v>442</v>
+        <v>568</v>
       </c>
       <c r="L128">
         <v>1</v>
@@ -10009,7 +10133,7 @@
         <v>45</v>
       </c>
       <c r="S128" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T128">
         <v>4</v>
@@ -10047,10 +10171,10 @@
         <v>44</v>
       </c>
       <c r="J129" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K129" s="12" t="s">
-        <v>442</v>
+        <v>567</v>
       </c>
       <c r="L129">
         <v>1</v>
@@ -10074,7 +10198,7 @@
         <v>45</v>
       </c>
       <c r="S129" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T129">
         <v>5</v>
@@ -10115,10 +10239,10 @@
         <v>44</v>
       </c>
       <c r="J130" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K130" s="12" t="s">
-        <v>442</v>
+        <v>565</v>
       </c>
       <c r="L130">
         <v>1</v>
@@ -10142,7 +10266,7 @@
         <v>45</v>
       </c>
       <c r="S130" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T130">
         <v>4</v>
@@ -10183,10 +10307,10 @@
         <v>44</v>
       </c>
       <c r="J131" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K131" s="12" t="s">
-        <v>442</v>
+        <v>566</v>
       </c>
       <c r="L131">
         <v>1</v>
@@ -10210,7 +10334,7 @@
         <v>45</v>
       </c>
       <c r="S131" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T131">
         <v>5</v>
@@ -10251,10 +10375,10 @@
         <v>44</v>
       </c>
       <c r="J132" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K132" s="12" t="s">
-        <v>442</v>
+        <v>564</v>
       </c>
       <c r="L132">
         <v>1</v>
@@ -10278,7 +10402,7 @@
         <v>45</v>
       </c>
       <c r="S132" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T132">
         <v>4</v>
@@ -10319,10 +10443,10 @@
         <v>44</v>
       </c>
       <c r="J133" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K133" s="12" t="s">
-        <v>442</v>
+        <v>563</v>
       </c>
       <c r="L133">
         <v>1</v>
@@ -10346,7 +10470,7 @@
         <v>45</v>
       </c>
       <c r="S133" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T133">
         <v>5</v>
@@ -10390,10 +10514,10 @@
         <v>44</v>
       </c>
       <c r="J134" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K134" s="12" t="s">
-        <v>442</v>
+        <v>562</v>
       </c>
       <c r="L134">
         <v>1</v>
@@ -10417,7 +10541,7 @@
         <v>45</v>
       </c>
       <c r="S134" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T134">
         <v>5</v>
@@ -10461,10 +10585,10 @@
         <v>44</v>
       </c>
       <c r="J135" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K135" s="12" t="s">
-        <v>442</v>
+        <v>561</v>
       </c>
       <c r="L135">
         <v>1</v>
@@ -10488,7 +10612,7 @@
         <v>45</v>
       </c>
       <c r="S135" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T135">
         <v>5</v>
@@ -10532,10 +10656,10 @@
         <v>44</v>
       </c>
       <c r="J136" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K136" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L136">
         <v>1</v>
@@ -10559,7 +10683,7 @@
         <v>45</v>
       </c>
       <c r="S136" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T136">
         <v>5</v>
@@ -10603,10 +10727,10 @@
         <v>44</v>
       </c>
       <c r="J137" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K137" s="12" t="s">
-        <v>442</v>
+        <v>560</v>
       </c>
       <c r="L137">
         <v>1</v>
@@ -10630,7 +10754,7 @@
         <v>45</v>
       </c>
       <c r="S137" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T137">
         <v>5</v>
@@ -10674,10 +10798,10 @@
         <v>44</v>
       </c>
       <c r="J138" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K138" s="12" t="s">
-        <v>442</v>
+        <v>559</v>
       </c>
       <c r="L138">
         <v>1</v>
@@ -10701,7 +10825,7 @@
         <v>45</v>
       </c>
       <c r="S138" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T138">
         <v>4</v>
@@ -10745,10 +10869,10 @@
         <v>44</v>
       </c>
       <c r="J139" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K139" s="12" t="s">
-        <v>442</v>
+        <v>558</v>
       </c>
       <c r="L139">
         <v>1</v>
@@ -10772,7 +10896,7 @@
         <v>45</v>
       </c>
       <c r="S139" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T139">
         <v>5</v>
@@ -10813,10 +10937,10 @@
         <v>44</v>
       </c>
       <c r="J140" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K140" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L140">
         <v>1</v>
@@ -10840,7 +10964,7 @@
         <v>45</v>
       </c>
       <c r="S140" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T140">
         <v>5</v>
@@ -10881,10 +11005,10 @@
         <v>44</v>
       </c>
       <c r="J141" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K141" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L141">
         <v>1</v>
@@ -10908,7 +11032,7 @@
         <v>45</v>
       </c>
       <c r="S141" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T141">
         <v>5</v>
@@ -10949,10 +11073,10 @@
         <v>44</v>
       </c>
       <c r="J142" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K142" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="L142">
         <v>1</v>
@@ -10976,7 +11100,7 @@
         <v>45</v>
       </c>
       <c r="S142" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T142">
         <v>5</v>
@@ -11017,10 +11141,10 @@
         <v>44</v>
       </c>
       <c r="J143" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K143" s="12" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="L143">
         <v>1</v>
@@ -11044,7 +11168,7 @@
         <v>45</v>
       </c>
       <c r="S143" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T143">
         <v>4</v>
@@ -11087,7 +11211,12 @@
       <c r="I144" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J144" s="13"/>
+      <c r="J144" s="13" t="s">
+        <v>612</v>
+      </c>
+      <c r="K144" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="L144">
         <v>1</v>
       </c>
@@ -11110,7 +11239,7 @@
         <v>373</v>
       </c>
       <c r="S144" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T144">
         <v>9</v>
@@ -11145,10 +11274,10 @@
         <v>44</v>
       </c>
       <c r="J145" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K145" s="12" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="L145">
         <v>1</v>
@@ -11172,7 +11301,7 @@
         <v>45</v>
       </c>
       <c r="S145" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T145">
         <v>9</v>
@@ -11216,10 +11345,10 @@
         <v>44</v>
       </c>
       <c r="J146" s="13" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K146" s="12" t="s">
-        <v>509</v>
+        <v>555</v>
       </c>
       <c r="L146">
         <v>1</v>
@@ -11243,7 +11372,7 @@
         <v>45</v>
       </c>
       <c r="S146" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T146">
         <v>9</v>
@@ -11287,10 +11416,10 @@
         <v>44</v>
       </c>
       <c r="J147" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K147" s="12" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L147">
         <v>1</v>
@@ -11314,7 +11443,7 @@
         <v>45</v>
       </c>
       <c r="S147" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T147">
         <v>5</v>
@@ -11352,10 +11481,10 @@
         <v>44</v>
       </c>
       <c r="J148" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K148" s="12" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L148">
         <v>1</v>
@@ -11379,7 +11508,7 @@
         <v>45</v>
       </c>
       <c r="S148" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T148">
         <v>9</v>
@@ -11420,10 +11549,10 @@
         <v>44</v>
       </c>
       <c r="J149" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K149" s="12" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="L149">
         <v>1</v>
@@ -11447,7 +11576,7 @@
         <v>45</v>
       </c>
       <c r="S149" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T149">
         <v>9</v>
@@ -11488,10 +11617,10 @@
         <v>44</v>
       </c>
       <c r="J150" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K150" s="12" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="L150">
         <v>1</v>
@@ -11515,7 +11644,7 @@
         <v>45</v>
       </c>
       <c r="S150" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T150">
         <v>9</v>
@@ -11559,10 +11688,10 @@
         <v>44</v>
       </c>
       <c r="J151" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K151" s="12" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="L151">
         <v>1</v>
@@ -11586,7 +11715,7 @@
         <v>45</v>
       </c>
       <c r="S151" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T151">
         <v>9</v>
@@ -11627,10 +11756,10 @@
         <v>44</v>
       </c>
       <c r="J152" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K152" s="12" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="L152">
         <v>1</v>
@@ -11654,7 +11783,7 @@
         <v>45</v>
       </c>
       <c r="S152" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T152">
         <v>9</v>
@@ -11698,10 +11827,10 @@
         <v>44</v>
       </c>
       <c r="J153" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K153" s="12" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="L153">
         <v>1</v>
@@ -11725,7 +11854,7 @@
         <v>45</v>
       </c>
       <c r="S153" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T153">
         <v>9</v>
@@ -11769,10 +11898,10 @@
         <v>44</v>
       </c>
       <c r="J154" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K154" s="12" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="L154">
         <v>1</v>
@@ -11796,7 +11925,7 @@
         <v>45</v>
       </c>
       <c r="S154" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T154">
         <v>9</v>
@@ -11837,10 +11966,10 @@
         <v>44</v>
       </c>
       <c r="J155" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K155" s="12" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="L155">
         <v>1</v>
@@ -11864,7 +11993,7 @@
         <v>45</v>
       </c>
       <c r="S155" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T155">
         <v>9</v>
@@ -11905,10 +12034,10 @@
         <v>44</v>
       </c>
       <c r="J156" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K156" s="12" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="L156">
         <v>1</v>
@@ -11932,7 +12061,7 @@
         <v>45</v>
       </c>
       <c r="S156" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T156">
         <v>9</v>
@@ -11973,10 +12102,10 @@
         <v>44</v>
       </c>
       <c r="J157" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K157" s="12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="L157">
         <v>1</v>
@@ -12000,7 +12129,7 @@
         <v>45</v>
       </c>
       <c r="S157" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T157">
         <v>9</v>
@@ -12041,10 +12170,10 @@
         <v>44</v>
       </c>
       <c r="J158" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K158" s="12" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="L158">
         <v>1</v>
@@ -12068,7 +12197,7 @@
         <v>45</v>
       </c>
       <c r="S158" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T158">
         <v>9</v>
@@ -12109,10 +12238,10 @@
         <v>44</v>
       </c>
       <c r="J159" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K159" s="12" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="L159">
         <v>1</v>
@@ -12136,7 +12265,7 @@
         <v>45</v>
       </c>
       <c r="S159" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T159">
         <v>9</v>
@@ -12177,10 +12306,10 @@
         <v>44</v>
       </c>
       <c r="J160" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K160" s="12" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="L160">
         <v>1</v>
@@ -12204,7 +12333,7 @@
         <v>45</v>
       </c>
       <c r="S160" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T160">
         <v>9</v>
@@ -12245,10 +12374,10 @@
         <v>44</v>
       </c>
       <c r="J161" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K161" s="12" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="L161">
         <v>1</v>
@@ -12272,7 +12401,7 @@
         <v>45</v>
       </c>
       <c r="S161" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T161">
         <v>9</v>
@@ -12313,10 +12442,10 @@
         <v>44</v>
       </c>
       <c r="J162" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K162" s="12" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="L162">
         <v>1</v>
@@ -12340,7 +12469,7 @@
         <v>45</v>
       </c>
       <c r="S162" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T162">
         <v>9</v>
@@ -12381,10 +12510,10 @@
         <v>44</v>
       </c>
       <c r="J163" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K163" s="12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="L163">
         <v>1</v>
@@ -12408,7 +12537,7 @@
         <v>45</v>
       </c>
       <c r="S163" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T163">
         <v>9</v>
@@ -12452,10 +12581,10 @@
         <v>44</v>
       </c>
       <c r="J164" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K164" s="12" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="L164">
         <v>1</v>
@@ -12479,7 +12608,7 @@
         <v>45</v>
       </c>
       <c r="S164" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T164">
         <v>9</v>
@@ -12520,10 +12649,10 @@
         <v>44</v>
       </c>
       <c r="J165" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K165" s="12" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="L165">
         <v>1</v>
@@ -12547,7 +12676,7 @@
         <v>45</v>
       </c>
       <c r="S165" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T165">
         <v>9</v>
@@ -12588,10 +12717,10 @@
         <v>44</v>
       </c>
       <c r="J166" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K166" s="12" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="L166">
         <v>1</v>
@@ -12615,7 +12744,7 @@
         <v>45</v>
       </c>
       <c r="S166" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T166">
         <v>9</v>
@@ -12656,10 +12785,10 @@
         <v>44</v>
       </c>
       <c r="J167" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K167" s="12" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="L167">
         <v>1</v>
@@ -12683,7 +12812,7 @@
         <v>45</v>
       </c>
       <c r="S167" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T167">
         <v>9</v>
@@ -12727,10 +12856,10 @@
         <v>44</v>
       </c>
       <c r="J168" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K168" s="12" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="L168">
         <v>1</v>
@@ -12754,7 +12883,7 @@
         <v>45</v>
       </c>
       <c r="S168" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T168">
         <v>9</v>
@@ -12795,10 +12924,10 @@
         <v>44</v>
       </c>
       <c r="J169" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K169" s="12" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="L169">
         <v>1</v>
@@ -12822,7 +12951,7 @@
         <v>45</v>
       </c>
       <c r="S169" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T169">
         <v>9</v>
@@ -12863,10 +12992,10 @@
         <v>44</v>
       </c>
       <c r="J170" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K170" s="12" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="L170">
         <v>1</v>
@@ -12890,7 +13019,7 @@
         <v>45</v>
       </c>
       <c r="S170" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T170">
         <v>9</v>
@@ -12934,10 +13063,10 @@
         <v>44</v>
       </c>
       <c r="J171" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K171" s="12" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="L171">
         <v>1</v>
@@ -12961,7 +13090,7 @@
         <v>45</v>
       </c>
       <c r="S171" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T171">
         <v>9</v>
@@ -13002,10 +13131,10 @@
         <v>44</v>
       </c>
       <c r="J172" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K172" s="12" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="L172">
         <v>1</v>
@@ -13029,7 +13158,7 @@
         <v>45</v>
       </c>
       <c r="S172" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T172">
         <v>9</v>
@@ -13070,11 +13199,11 @@
         <v>44</v>
       </c>
       <c r="J173" s="13" t="s">
+        <v>549</v>
+      </c>
+      <c r="K173" s="12" t="s">
         <v>553</v>
       </c>
-      <c r="K173" s="12" t="s">
-        <v>536</v>
-      </c>
       <c r="L173">
         <v>1</v>
       </c>
@@ -13097,7 +13226,7 @@
         <v>45</v>
       </c>
       <c r="S173" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T173">
         <v>9</v>
@@ -13138,10 +13267,10 @@
         <v>44</v>
       </c>
       <c r="J174" s="13" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="K174" s="12" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="L174">
         <v>1</v>
@@ -13165,7 +13294,7 @@
         <v>45</v>
       </c>
       <c r="S174" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T174">
         <v>9</v>

</xml_diff>